<commit_message>
Fungsi import image mahasiswa
</commit_message>
<xml_diff>
--- a/Menu Data Mahasiswa.xlsx
+++ b/Menu Data Mahasiswa.xlsx
@@ -1,21 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22430"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\lara-kelulusan\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{408A1F89-C3FB-46A2-A131-B7810A2555A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Laporan Data Mahasiswa" sheetId="1" r:id="rId4"/>
+    <sheet name="Laporan Data Mahasiswa" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="999999" calcMode="auto" calcCompleted="1" fullCalcOnLoad="0" forceFullCalc="0"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="39">
   <si>
     <t>Laporan Data Mahasiswa</t>
   </si>
@@ -137,32 +142,21 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
-  <numFmts count="0"/>
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <b val="1"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
+      <b/>
       <sz val="18"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <b val="1"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -173,64 +167,125 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="2">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
-        <color rgb="000"/>
+        <color rgb="FF000000"/>
       </left>
       <right style="thin">
-        <color rgb="000"/>
+        <color rgb="FF000000"/>
       </right>
       <top style="thin">
-        <color rgb="000"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
-        <color rgb="000"/>
+        <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" fontId="2" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" fontId="2" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="2" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1028701</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>606712</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B945F8B-294B-4F93-A9CF-68FC2FE68C59}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1381125" y="1057274"/>
+          <a:ext cx="809626" cy="606713"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -519,344 +574,230 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
-  <dimension ref="A1:P9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A2:P7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A9" sqref="A9:P9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.570313" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="12.854004" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="10.568848" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="19.995117" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="15.281982" bestFit="true" customWidth="true" style="0"/>
-    <col min="6" max="6" width="16.424561" bestFit="true" customWidth="true" style="0"/>
-    <col min="7" max="7" width="6.998291" bestFit="true" customWidth="true" style="0"/>
-    <col min="8" max="8" width="15.281982" bestFit="true" customWidth="true" style="0"/>
-    <col min="9" max="9" width="16.424561" bestFit="true" customWidth="true" style="0"/>
-    <col min="10" max="10" width="12.854004" bestFit="true" customWidth="true" style="0"/>
-    <col min="11" max="11" width="16.424561" bestFit="true" customWidth="true" style="0"/>
-    <col min="12" max="12" width="22.280273" bestFit="true" customWidth="true" style="0"/>
-    <col min="13" max="13" width="23.422852" bestFit="true" customWidth="true" style="0"/>
-    <col min="14" max="14" width="12.854004" bestFit="true" customWidth="true" style="0"/>
-    <col min="15" max="15" width="12.854004" bestFit="true" customWidth="true" style="0"/>
-    <col min="16" max="16" width="17.567139" bestFit="true" customWidth="true" style="0"/>
+    <col min="1" max="1" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" customWidth="1"/>
+    <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:16">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
     </row>
-    <row r="4" spans="1:16">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="4" t="s">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="4" t="s">
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="3"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="2"/>
     </row>
-    <row r="5" spans="1:16">
-      <c r="A5" s="5" t="s">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="I5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="J5" s="5" t="s">
+      <c r="J5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="K5" s="5" t="s">
+      <c r="K5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="L5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="M5" s="2" t="s">
+      <c r="M5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N5" s="2" t="s">
+      <c r="N5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="O5" s="5" t="s">
+      <c r="O5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="P5" s="7" t="s">
+      <c r="P5" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
-      <c r="A6" s="6">
+    <row r="6" spans="1:16" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
         <v>1</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="2">
         <v>1819117641</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2"/>
+      <c r="D6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="P6" s="4">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>2</v>
+      </c>
+      <c r="B7" s="2">
+        <v>1819117642</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="3" t="s">
+      <c r="D7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G6" s="6" t="s">
+      <c r="F7" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="I6" s="6" t="s">
+      <c r="I7" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="J6" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="L6" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="M6" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="N6" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="O6" s="3" t="s">
+      <c r="J7" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="O7" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="P6" s="6">
-        <v>2021</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16">
-      <c r="A7" s="6">
-        <v>2</v>
-      </c>
-      <c r="B7" s="3">
-        <v>1819117642</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="I7" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="J7" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="L7" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="M7" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="N7" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="O7" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="P7" s="6">
-        <v>2020</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16">
-      <c r="A8" s="6">
-        <v>3</v>
-      </c>
-      <c r="B8" s="3">
-        <v>1819117641</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="I8" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="J8" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="K8" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="L8" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="M8" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="N8" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="O8" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="P8" s="6">
-        <v>2021</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16">
-      <c r="A9" s="6">
-        <v>4</v>
-      </c>
-      <c r="B9" s="3">
-        <v>1819117642</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="I9" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="J9" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="K9" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="L9" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="M9" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="N9" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="O9" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="P9" s="6">
+      <c r="P7" s="4">
         <v>2020</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
-  <mergeCells>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <mergeCells count="3">
     <mergeCell ref="A2:O2"/>
     <mergeCell ref="D4:H4"/>
     <mergeCell ref="L4:N4"/>
   </mergeCells>
-  <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
+  <pageSetup fitToWidth="0" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>